<commit_message>
*modify video and grid
</commit_message>
<xml_diff>
--- a/source/GridForIteration2-3004-F18.xlsx
+++ b/source/GridForIteration2-3004-F18.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="155">
   <si>
     <t>actual</t>
   </si>
@@ -583,6 +583,10 @@
   </si>
   <si>
     <t>no</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>AllAI</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -1308,7 +1312,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="75" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="75" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
@@ -1968,7 +1972,9 @@
       <c r="A59" t="s">
         <v>23</v>
       </c>
-      <c r="B59" s="7"/>
+      <c r="B59" s="7" t="s">
+        <v>154</v>
+      </c>
       <c r="C59" s="1" t="s">
         <v>114</v>
       </c>

</xml_diff>